<commit_message>
Updated results and readme files
</commit_message>
<xml_diff>
--- a/autoencoder_coral_mini/Results.xlsx
+++ b/autoencoder_coral_mini/Results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mahdi\Documents\GitHub\tensorflow-lite-microcontroller-autoencoder\autoencoder_coral_mini\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C728607-3429-4F21-9A2E-1711385143C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B5B5165-0ABB-42A1-8B20-AC650F6C3CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="14">
-  <si>
-    <t>Total Inference Time (seconds)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
   <si>
     <t>ID</t>
   </si>
@@ -53,12 +50,6 @@
     <t>Running run_tflite on Coral Mini Dev CPU</t>
   </si>
   <si>
-    <t xml:space="preserve">Before running </t>
-  </si>
-  <si>
-    <t xml:space="preserve">While running </t>
-  </si>
-  <si>
     <t>Power Measurements on Coral Dev Mini</t>
   </si>
   <si>
@@ -71,20 +62,47 @@
     <t>PBUS (W)</t>
   </si>
   <si>
-    <t>Differences (While Running - Before Running)</t>
-  </si>
-  <si>
     <t>Running run_tflite on PC</t>
   </si>
   <si>
     <t>PC Processor: Intel® Core ™ i7-1075 CPU @ 2.60GHz. 2592 Mhz, 6 Cores, 12 Logical Processors</t>
+  </si>
+  <si>
+    <t>While running inference</t>
+  </si>
+  <si>
+    <t>Differences = While Running - Before Running</t>
+  </si>
+  <si>
+    <t>voltage drop of -0.02</t>
+  </si>
+  <si>
+    <t>current increase of 150 mA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">power increase of 730 mW </t>
+  </si>
+  <si>
+    <t>Before running inference</t>
+  </si>
+  <si>
+    <t>Total Inference Time (seconds) (1712 samples)</t>
+  </si>
+  <si>
+    <t>Individual sample inference time (coral mini) (seconds)</t>
+  </si>
+  <si>
+    <t>Individual sample inference time (PC) (seconds)</t>
+  </si>
+  <si>
+    <t>single inference time in msec</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -115,6 +133,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF002060"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="9" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -136,7 +184,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -153,13 +201,28 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -442,17 +505,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K32"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.42578125" style="2" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.140625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="27.85546875" style="2" customWidth="1"/>
     <col min="4" max="4" width="8.28515625" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.140625" style="2" customWidth="1"/>
     <col min="6" max="6" width="7.7109375" style="2" customWidth="1"/>
@@ -460,291 +523,337 @@
     <col min="8" max="8" width="7.140625" style="2" customWidth="1"/>
     <col min="9" max="9" width="7" style="2" customWidth="1"/>
     <col min="10" max="10" width="13.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="49.28515625" style="2" customWidth="1"/>
+    <col min="11" max="11" width="45.28515625" style="2" customWidth="1"/>
     <col min="12" max="12" width="45.7109375" style="2" customWidth="1"/>
     <col min="13" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="39" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" ht="39" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C2" s="2">
         <v>28.42</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="6"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="2">
+        <f>C5/1712</f>
+        <v>1.6592679127725857E-2</v>
+      </c>
+      <c r="L2" s="5">
+        <f>K2*1000</f>
+        <v>16.592679127725855</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C3" s="2">
         <v>28.37</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="2">
+        <f>C9/1712</f>
+        <v>5.2764797507788162E-4</v>
+      </c>
+      <c r="L3" s="5">
+        <f>K3*1000</f>
+        <v>0.52764797507788164</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C4" s="2">
         <v>28.43</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C5" s="4">
         <f>AVERAGE(C2:C4)</f>
         <v>28.406666666666666</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C6" s="2">
         <v>0.89</v>
       </c>
-      <c r="D6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="8"/>
-      <c r="I6" s="8"/>
-      <c r="J6" s="8"/>
-      <c r="K6" s="8"/>
-    </row>
-    <row r="7" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:12" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>2</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C7" s="2">
         <v>0.92</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="C8" s="2">
         <v>0.9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C9" s="4">
         <f>AVERAGE(C6:C8)</f>
         <v>0.90333333333333332</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="1" t="s">
+    <row r="10" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:12" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="9">
+        <v>5.0599999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="9">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C14" s="9">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C15" s="5"/>
+    </row>
+    <row r="16" spans="1:12" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="12" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2">
-        <v>5.0599999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="2">
-        <v>0.17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C14" s="2">
-        <v>0.87</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="5"/>
-    </row>
-    <row r="16" spans="1:11" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C17" s="2">
+      <c r="C17" s="12">
         <v>5.04</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="12">
         <v>5.04</v>
       </c>
-      <c r="E17" s="2">
+      <c r="E17" s="12">
         <v>5.04</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="12">
         <v>5.04</v>
       </c>
-      <c r="G17" s="2">
+      <c r="G17" s="12">
         <v>5.04</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="12">
         <v>5.04</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="12">
         <v>5.04</v>
       </c>
-      <c r="J17" s="4">
+      <c r="J17" s="13">
         <f>AVERAGE(C17:I17)</f>
         <v>5.04</v>
       </c>
-      <c r="K17" s="5">
+      <c r="K17" s="13">
         <f>J17-C12</f>
         <v>-1.9999999999999574E-2</v>
       </c>
-    </row>
-    <row r="18" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="2">
+      <c r="L17" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18" s="12">
         <v>0.33</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E18" s="12">
         <v>0.28999999999999998</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="12">
         <v>0.3</v>
       </c>
-      <c r="G18" s="2">
+      <c r="G18" s="12">
         <v>0.31</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="12">
         <v>0.35</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="12">
         <v>0.34</v>
       </c>
-      <c r="J18" s="4">
+      <c r="J18" s="13">
         <f t="shared" ref="J18:J19" si="0">AVERAGE(C18:I18)</f>
         <v>0.31571428571428573</v>
       </c>
-      <c r="K18" s="5">
+      <c r="K18" s="13">
         <f>J18-C13</f>
         <v>0.14571428571428571</v>
       </c>
-    </row>
-    <row r="19" spans="2:11" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="2">
+      <c r="L18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C19" s="12">
         <v>1.66</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="12">
         <v>1.47</v>
       </c>
-      <c r="E19" s="2">
+      <c r="E19" s="12">
         <v>1.48</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="12">
         <v>1.53</v>
       </c>
-      <c r="G19" s="2">
+      <c r="G19" s="12">
         <v>1.58</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="12">
         <v>1.8</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="12">
         <v>1.71</v>
       </c>
-      <c r="J19" s="4">
+      <c r="J19" s="13">
         <f t="shared" si="0"/>
         <v>1.6042857142857143</v>
       </c>
-      <c r="K19" s="5">
+      <c r="K19" s="13">
         <f>J19-C14</f>
         <v>0.73428571428571432</v>
       </c>
-    </row>
-    <row r="20" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:11" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+      <c r="L19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:12" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C16:I16"/>
     <mergeCell ref="D6:K6"/>
+    <mergeCell ref="E2:J2"/>
+    <mergeCell ref="E3:J3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>